<commit_message>
Individual Sale & Model Names Improves
</commit_message>
<xml_diff>
--- a/BrandexSalesAdapter.ExcelLogic/wwwroot/UploadExcel/Sofarma-TESTxlsx.xlsx
+++ b/BrandexSalesAdapter.ExcelLogic/wwwroot/UploadExcel/Sofarma-TESTxlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Petar/Documents/Documents – Petar’s MacBook Pro/Firmata/Справка/TestForSfotware/2020 -СКЛАДОВЕ СПРАВКИ/7. СКЛАДОВЕ СПРАВКИ ЮЛИ 2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1517C3C-6286-BF42-8B80-2941E403EACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C727AEDB-230F-5942-8CD6-C3FC2706B6E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{2EA49580-10E5-4415-945F-B290E85E1788}"/>
   </bookViews>
@@ -542,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C751EB7-4EC1-47EC-90E3-2E95477D63BA}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:L7"/>
+    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -559,7 +559,7 @@
     <col min="9" max="9" width="43.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="38.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>